<commit_message>
modify db and api
</commit_message>
<xml_diff>
--- a/Specification file/銀行/個金行銷部/華南銀行-個金行銷部-房貸API欄位輸出文件_v1(回覆).xlsx
+++ b/Specification file/銀行/個金行銷部/華南銀行-個金行銷部-房貸API欄位輸出文件_v1(回覆).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B68F398-46D3-174C-9AC7-9A62724B3FB3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94C8602-E7AE-8E4E-BD4C-F0A5EF263E85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="2240" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="153">
   <si>
     <t>Field</t>
   </si>
@@ -647,10 +647,6 @@
   </si>
   <si>
     <t>請確認信用分級之所有種類以及分佈</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>creadit_level</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -1032,6 +1028,14 @@
   <si>
     <t>正擔保 60% 
 加強債權 40%</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>credit_level</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1752,7 +1756,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1800,10 +1804,10 @@
         <v>29</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="301" thickBot="1">
@@ -1826,7 +1830,7 @@
         <v>31</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="343" thickBot="1">
@@ -1843,13 +1847,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>90</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="121" thickBot="1">
@@ -1863,16 +1867,16 @@
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" thickBot="1">
@@ -1892,10 +1896,10 @@
         <v>33</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="76" thickBot="1">
@@ -1909,7 +1913,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>34</v>
@@ -1918,7 +1922,7 @@
         <v>35</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="91" thickBot="1">
@@ -1941,15 +1945,15 @@
         <v>15</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="166" thickBot="1">
       <c r="A9" s="8" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
@@ -1964,7 +1968,7 @@
         <v>92</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2035,7 +2039,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="91" thickBot="1">
@@ -2055,10 +2059,10 @@
         <v>59</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="46" thickBot="1">
@@ -2072,16 +2076,16 @@
         <v>4</v>
       </c>
       <c r="D4" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>132</v>
       </c>
       <c r="F4" s="36" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="121" thickBot="1">
@@ -2104,7 +2108,7 @@
         <v>11</v>
       </c>
       <c r="G5" s="43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="121" thickBot="1">
@@ -2127,7 +2131,7 @@
         <v>62</v>
       </c>
       <c r="G6" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="46" thickBot="1">
@@ -2150,7 +2154,7 @@
         <v>11</v>
       </c>
       <c r="G7" s="43" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="91" thickBot="1">
@@ -2173,7 +2177,7 @@
         <v>65</v>
       </c>
       <c r="G8" s="43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="61" thickBot="1">
@@ -2196,7 +2200,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="46" thickBot="1">
@@ -2219,7 +2223,7 @@
         <v>68</v>
       </c>
       <c r="G10" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="46" thickBot="1">
@@ -2242,12 +2246,12 @@
         <v>11</v>
       </c>
       <c r="G11" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="61" thickBot="1">
       <c r="A12" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>6</v>
@@ -2256,7 +2260,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>99</v>
@@ -2265,7 +2269,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="61" thickBot="1">
@@ -2288,7 +2292,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31" thickBot="1">
@@ -2302,7 +2306,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E14" s="34" t="s">
         <v>70</v>
@@ -2331,7 +2335,7 @@
         <v>73</v>
       </c>
       <c r="G15" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="46" thickBot="1">
@@ -2345,16 +2349,16 @@
         <v>4</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>74</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G16" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="31" thickBot="1">
@@ -2368,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>75</v>
@@ -2391,7 +2395,7 @@
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -2442,7 +2446,7 @@
         <v>84</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="91" thickBot="1">
@@ -2462,10 +2466,10 @@
         <v>83</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="35" thickBot="1">
@@ -2488,7 +2492,7 @@
         <v>94</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="343" thickBot="1">
@@ -2511,7 +2515,7 @@
         <v>90</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="136" thickBot="1">
@@ -2534,7 +2538,7 @@
         <v>87</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="61" thickBot="1">
@@ -2548,7 +2552,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>89</v>
@@ -2557,7 +2561,7 @@
         <v>88</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="76" thickBot="1">
@@ -2574,13 +2578,13 @@
         <v>97</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>98</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>